<commit_message>
files move from voice\wav to voice
</commit_message>
<xml_diff>
--- a/master.xlsx
+++ b/master.xlsx
@@ -381,7 +381,7 @@
   <dimension ref="A1:C64"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -403,13 +403,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B2" s="1">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>